<commit_message>
1# removed bidirectional, 2# added sample photo to ExcelDinner, 3# still don't working all ManyToMany ralations
</commit_message>
<xml_diff>
--- a/ExcelReader/src/main/resource/jadlospis2.xlsx
+++ b/ExcelReader/src/main/resource/jadlospis2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\eatMeAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\eatmeall\ExcelReader\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E130790C-F803-4B3A-B74B-1673F123B1FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED744BCA-9832-4930-A3E4-38CFC7225D6D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="175">
-  <si>
-    <t>ŚNIADANIE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="172">
   <si>
     <t>Koktajl mleczny z otrębami</t>
   </si>
@@ -63,9 +60,6 @@
     <t>1 szklanka</t>
   </si>
   <si>
-    <t>Sniadanie</t>
-  </si>
-  <si>
     <t>Jogurt owocowy z suszonymi owocami</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>3 szt.</t>
   </si>
   <si>
-    <t>Śniadanie</t>
-  </si>
-  <si>
     <t>Drobiowa pancetta na grzance z jajkiem</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>1sz.</t>
   </si>
   <si>
-    <t>Bułkę kajzerkę przekroić na pół, wyciągnąć miąższ ze środka, posmarować cienko margaryną (cienko!) i włożyć do tostera. Na patelni przygotować 2 małe jajka sadzone, posolić, popieprzyć. Na grzankach w zagłębieniu położyć po plasterku szynki z kurczaka, na nich położyć jajko sadzone. Całość obficie posypać szczypiorkiem. Podawać z pomidorkami koktajlowymi.</t>
-  </si>
-  <si>
     <t>Jajko</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>1/3 szklanki</t>
   </si>
   <si>
-    <t>Rano wymieszać: sok z czarnej porzeczki, mleko 2% tł, jogurt naturalny, płatki owsiane, miód, schłodzić w lodówce. Przed zjedzeniem dodać orzechy włoskie</t>
-  </si>
-  <si>
     <t>mleko 2%</t>
   </si>
   <si>
@@ -192,9 +177,6 @@
     <t>1 szt.</t>
   </si>
   <si>
-    <t xml:space="preserve">Na patelni teflonowej na maśle wbić wymieszane jajko z białkami doprawić solą i pieprzem, dodać szczypiorek, zjeść z chlebem i pomidorem pokrojonym w ćwiartki. </t>
-  </si>
-  <si>
     <t>tylko białko</t>
   </si>
   <si>
@@ -210,9 +192,6 @@
     <t>1 duzy</t>
   </si>
   <si>
-    <t>Lunch</t>
-  </si>
-  <si>
     <t>Chleb żytni razowy Do przegryzania wafle ryżowe</t>
   </si>
   <si>
@@ -300,9 +279,6 @@
     <t>Filet z piersi kurczaka</t>
   </si>
   <si>
-    <t>Filet z piersi kurczaka pokroić na kawałki, przyprawić solą, pieprzem i podsmażyć na patelni grillowej. Pokrojone pieczarki poddusić z solą na oleju rzepakowym, dodać fasolkę szparagową i startą drobno marchewkę. Dodać piersi z kurczaka, przyprawić ulubionymi ziołami, dodać natkę pietruszki. Podawać z ugotowaną kaszą gryczaną z jogurtem naturalnym wymieszanym z pietruszką.</t>
-  </si>
-  <si>
     <t>pieczarki</t>
   </si>
   <si>
@@ -339,9 +315,6 @@
     <t>kolka liści</t>
   </si>
   <si>
-    <t>1# Przygotować surówkę: białą kapustę (150 g, kilka liści) pokroić cienko, zmorzyć solą, odstawić na kilka minut. Następnie dodać oliwę z oliwek (5 g, 1 łyżeczka), doprawić solą, pieprzem i oregano. 2# Bułkę do hamburgerów (55 g, 1 szt) [można zastąpić zwykłą bułką pszenną 60 g, średnia szt] posmarować z dwóch stron sosem czosnkowym (majonez light 8 g, 1 łyżeczka, jogurt naturalny 40 g, 2 łyżki czosnek) i keczupem (8 g, 1 łyżeczka). Na jednej połówce ułożyć pokrojone warzywa: paprykę czerwoną (15 g, kilka pasków), żółtą (15 g, kilka plastrów) i sałatę (duży liść). Przygotować mięso: zmielone mięso z piersi z kurczaka 75 g) wymieszać z pokrojoną cebulą (30 g, ¼ szt), białkiem jaja (białko z 1 jaja) i namoczoną w wodzie bułką (20 g, 1/3 szt), doprawić do smaku solą, pieprzem i np. papryką ostrą. Smażyć na patelni grillowej do rumianego koloru.</t>
-  </si>
-  <si>
     <t>oliwę z oliwek</t>
   </si>
   <si>
@@ -399,9 +372,6 @@
     <t>Schab bez kości</t>
   </si>
   <si>
-    <t>Schab bez kości (100 g, 1 plaster), ser żółty (10 g, 1 mały plaster), papryka czerwona (2 plasterki), sól, pieprz, papryka słodka. Ziemniaki (200 g, 2 duże szt), pietruszka natka według uznania. Surówka gotowa np. Grześkowiak (180 g, ½ większego opakowania). Do picia sok pomidorowy (200 ml, 1 szkl). Schab rozbić na cienki kotlet, doprawić przyprawami, do środka włożyć ser żółty i paprykę, zawinąć w roladkę. Folię aluminiową bardzo delikatnie posmarować olejem, zawinąć w nią roladkę i zapiekać w piekarniku nagrzanym do 220°C, około 30-40 min. Podawać z ugotowanymi ziemniakami posypanymi pietruszką i surówką.</t>
-  </si>
-  <si>
     <t>ser żółty</t>
   </si>
   <si>
@@ -492,9 +462,6 @@
     <t>1/5 opak</t>
   </si>
   <si>
-    <t xml:space="preserve">Ugotować ryż wymieszać z mięsem mielonym z indyka, białkiem jaja i natką pietruszki, przyprawić solą i pieprzem. Farszem wypełnić paprykę czerwoną. Podlać 1 łyżką wody/bulionu. Zapiekać w piekarniku nagrzanym do 200 stopni ok. 30-40 min. 10 min przed końcem posypać starym żółtym serem. </t>
-  </si>
-  <si>
     <t>mięso mielone z kurczaka lub indyka</t>
   </si>
   <si>
@@ -550,6 +517,30 @@
   </si>
   <si>
     <t>Kwaśniewski</t>
+  </si>
+  <si>
+    <t>ugotować ryż; wymieszać z mięsem mielonym z indyka, białkiem jaja i natką pietruszki; przyprawić solą i pieprzem; farszem wypełnić paprykę czerwoną; podlać 1 łyżką wody/bulionu; zapiekać w piekarniku nagrzanym do 200 stopni ok. 30-40 min; 10 min przed końcem posypać starym żółtym serem</t>
+  </si>
+  <si>
+    <t>Bułkę kajzerkę przekroić na pół; wyciągnąć miąższ ze środka; posmarować cienko margaryną (cienko!) i włożyć do tostera; na patelni przygotować 2 małe jajka sadzone, posolić, popieprzyć; na grzankach w zagłębieniu położyć po plasterku szynki z kurczaka, na nich położyć jajko sadzone; całość obficie posypać szczypiorkiem; podawać z pomidorkami koktajlowymi.</t>
+  </si>
+  <si>
+    <t>Rano wymieszać: sok z czarnej porzeczki, mleko 2% tł, jogurt naturalny, płatki owsiane, miód; schłodzić w lodówce.; przed zjedzeniem dodać orzechy włoskie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na patelni teflonowej na maśle wbić wymieszane jajko z białkami; doprawić solą i pieprzem ; dodać szczypiorek; zjeść z chlebem i pomidorem pokrojonym w ćwiartki. </t>
+  </si>
+  <si>
+    <t>Filet z piersi kurczaka pokroić na kawałki; przyprawić solą, pieprzem i podsmażyć na patelni grillowej; pokrojone pieczarki poddusić z solą na oleju rzepakowym; dodać fasolkę szparagową i startą drobno marchewkę; dodać piersi z kurczaka, przyprawić ulubionymi ziołami; dodać natkę pietruszki. Podawać z ugotowaną kaszą gryczaną z jogurtem naturalnym wymieszanym z pietruszką.</t>
+  </si>
+  <si>
+    <t>Schab rozbić na cienki kotlet, doprawić przyprawami; do środka włożyć ser żółty i paprykę ; zawinąć w roladkę; folię aluminiową bardzo delikatnie posmarować olejem; zawinąć w nią roladkę i zapiekać w piekarniku nagrzanym do 220°C, około 30-40 min; podawać z ugotowanymi ziemniakami posypanymi pietruszką i surówką.</t>
+  </si>
+  <si>
+    <t>1# przygotować surówkę:; białą kapustę pokroić cienko;  zmorzyć solą, odstawić na kilka minut; następnie dodać oliwę z oliwek;  doprawić solą, pieprzem i oregano;  2# Bułkę do hamburgerów [można zastąpić zwykłą bułką pszenną 60 g, średnia szt]; posmarować z dwóch stron sosem czosnkowym i keczupem; na jednej połówce ułożyć pokrojone warzywa:;  paprykę czerwoną; żółtą  i sałatę;  przygotować mięso: zmielone mięso z piersi z kurczaka; wymieszać z pokrojoną cebulą, białkiem jaja i namoczoną w wodzie bułką; doprawić do smaku solą, pieprzem i np. papryką ostrą; smażyć na patelni grillowej do rumianego koloru.</t>
+  </si>
+  <si>
+    <t>śniadanie</t>
   </si>
 </sst>
 </file>
@@ -929,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,34 +936,34 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="C1" s="1">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="1">
         <v>400</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="J1" s="1">
         <v>300</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -981,16 +972,16 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1002,16 +993,16 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1023,16 +1014,16 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F4" s="1">
         <v>200</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1044,7 +1035,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1058,34 +1049,34 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1">
         <v>200</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1">
         <v>300</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1094,16 +1085,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1115,16 +1106,16 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
         <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1136,16 +1127,16 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1">
         <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1157,7 +1148,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1171,34 +1162,34 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1">
         <v>200</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1">
         <v>300</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1207,16 +1198,16 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1">
         <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1228,16 +1219,16 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1249,16 +1240,16 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1">
         <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1270,7 +1261,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1284,34 +1275,34 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="C16" s="1">
         <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="J16" s="1">
         <v>300</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1320,16 +1311,16 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1">
         <v>120</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1341,13 +1332,13 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F18" s="1">
         <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1360,16 +1351,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1">
         <v>20</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1381,16 +1372,16 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1">
         <v>75</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1402,7 +1393,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1416,34 +1407,34 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1">
         <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>41</v>
+        <v>166</v>
       </c>
       <c r="J22" s="1">
         <v>300</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1452,16 +1443,16 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F23" s="1">
         <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1473,16 +1464,16 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F24" s="1">
         <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1494,16 +1485,16 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F25" s="1">
         <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1515,16 +1506,16 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F26" s="1">
         <v>20</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1536,16 +1527,16 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1">
         <v>12</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1557,7 +1548,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1571,34 +1562,34 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F29" s="1">
         <v>75</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="J29" s="1">
         <v>300</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1607,16 +1598,16 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F30" s="1">
         <v>80</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1628,16 +1619,16 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F31" s="1">
         <v>100</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1649,16 +1640,16 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F32" s="1">
         <v>100</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1670,7 +1661,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1684,34 +1675,34 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1">
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F34" s="1">
         <v>50</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J34" s="1">
         <v>350</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1720,16 +1711,16 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F35" s="1">
         <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1741,16 +1732,16 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F36" s="1">
         <v>15</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1762,16 +1753,16 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F37" s="1">
         <v>15</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1783,16 +1774,16 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F38" s="1">
         <v>20</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1804,16 +1795,16 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F39" s="1">
         <v>150</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1825,7 +1816,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1839,34 +1830,34 @@
         <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1">
         <v>15</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F41" s="1">
         <v>160</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J41" s="1">
         <v>350</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1875,16 +1866,16 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F42" s="1">
         <v>30</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -1896,7 +1887,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1910,34 +1901,34 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C44" s="1">
         <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F44" s="1">
         <v>80</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J44" s="1">
         <v>350</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1946,16 +1937,16 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F45" s="1">
         <v>5</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -1967,16 +1958,16 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F46" s="1">
         <v>20</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -1988,16 +1979,16 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F47" s="1">
         <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2009,16 +2000,16 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F48" s="1">
         <v>50</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2030,7 +2021,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2044,34 +2035,34 @@
         <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1">
         <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F50" s="1">
         <v>200</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="J50" s="1">
         <v>300</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2080,16 +2071,16 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F51" s="1">
         <v>500</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2101,7 +2092,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2115,34 +2106,34 @@
         <v>11</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C53" s="1">
         <v>30</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F53" s="1">
         <v>200</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="J53" s="1">
         <v>300</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2151,16 +2142,16 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F54" s="1">
         <v>500</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2172,7 +2163,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2186,34 +2177,34 @@
         <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C56" s="1">
         <v>30</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F56" s="1">
         <v>200</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J56" s="1">
         <v>300</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2222,7 +2213,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2236,34 +2227,34 @@
         <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1">
         <v>45</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F58" s="1">
         <v>150</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>91</v>
+        <v>168</v>
       </c>
       <c r="J58" s="1">
         <v>600</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2272,16 +2263,16 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F59" s="1">
         <v>150</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -2293,16 +2284,16 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F60" s="1">
         <v>5</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -2314,16 +2305,16 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F61" s="1">
         <v>200</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -2335,16 +2326,16 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F62" s="1">
         <v>200</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2356,16 +2347,16 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F63" s="1">
         <v>75</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -2377,16 +2368,16 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F64" s="1">
         <v>75</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -2398,7 +2389,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2407,39 +2398,39 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>14</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C66" s="1">
         <v>45</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F66" s="1">
         <v>150</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="J66" s="1">
         <v>600</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2448,16 +2439,16 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -2469,16 +2460,16 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F68" s="1">
         <v>55</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -2490,16 +2481,16 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F69" s="1">
         <v>8</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -2511,16 +2502,16 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F70" s="1">
         <v>40</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
@@ -2532,12 +2523,12 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -2549,16 +2540,16 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F72" s="1">
         <v>8</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -2570,16 +2561,16 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F73" s="1">
         <v>15</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2591,12 +2582,12 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -2608,13 +2599,13 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F75" s="1">
         <v>75</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
@@ -2627,16 +2618,16 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F76" s="1">
         <v>30</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2648,16 +2639,16 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F77" s="1">
         <v>75</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2669,16 +2660,16 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F78" s="1">
         <v>20</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -2690,7 +2681,7 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2699,39 +2690,39 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>15</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1">
         <v>45</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F80" s="1">
         <v>100</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="J80" s="1">
         <v>600</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2740,16 +2731,16 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F81" s="1">
         <v>10</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2761,16 +2752,16 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F82" s="1">
         <v>30</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2782,16 +2773,16 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F83" s="1">
         <v>30</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2803,16 +2794,16 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F84" s="1">
         <v>200</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2824,12 +2815,12 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
@@ -2841,16 +2832,16 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F86" s="1">
         <v>100</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -2862,16 +2853,16 @@
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="F87" s="1">
         <v>200</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -2883,7 +2874,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -2897,34 +2888,34 @@
         <v>16</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C89" s="1">
         <v>10</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F89" s="1">
         <v>80</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="J89" s="1">
         <v>350</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2933,19 +2924,19 @@
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -2956,16 +2947,16 @@
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F91" s="1">
         <v>50</v>
       </c>
       <c r="G91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
@@ -2977,16 +2968,16 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F92" s="1">
         <v>30</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -2998,16 +2989,16 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F93" s="1">
         <v>50</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -3019,16 +3010,16 @@
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F94" s="1">
         <v>25</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -3040,16 +3031,16 @@
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F95" s="1">
         <v>100</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -3061,7 +3052,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -3075,34 +3066,34 @@
         <v>17</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C97" s="1">
         <v>10</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F97" s="1">
         <v>80</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="J97" s="1">
         <v>350</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3111,16 +3102,16 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F98" s="1">
         <v>20</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -3132,16 +3123,16 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F99" s="1">
         <v>30</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -3153,16 +3144,16 @@
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F100" s="1">
         <v>10</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -3174,12 +3165,12 @@
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
@@ -3191,16 +3182,16 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
@@ -3212,7 +3203,7 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -3226,34 +3217,34 @@
         <v>18</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C104" s="1">
         <v>20</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F104" s="1">
         <v>20</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="J104" s="1">
         <v>350</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -3262,16 +3253,16 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="F105" s="1">
         <v>65</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -3283,16 +3274,16 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F106" s="1">
         <v>75</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -3304,16 +3295,16 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F107" s="1">
         <v>220</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
@@ -3325,16 +3316,16 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F108" s="1">
         <v>10</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -3346,7 +3337,7 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>

</xml_diff>